<commit_message>
test Geneva get Country group total OK
</commit_message>
<xml_diff>
--- a/samples/SFC_report_20200430.xlsx
+++ b/samples/SFC_report_20200430.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhangst\git\risk_report\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A3F05F-35D8-4F84-A372-6270FCAC76FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5960EE21-A393-4F08-AA2D-6FD0A3047166}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{3B4425A6-A2F6-45C4-8461-7D72DCF5044F}"/>
   </bookViews>
@@ -981,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8183F8E1-FA4D-46EE-B2E4-AF8A3D48D85A}">
   <dimension ref="A2:T207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2930,8 +2930,8 @@
         <v>11361748.799019611</v>
       </c>
       <c r="F82" s="4">
-        <f t="shared" si="0"/>
-        <v>49267942.098813206</v>
+        <f>F81</f>
+        <v>15742145.411506709</v>
       </c>
       <c r="G82" s="4">
         <f t="shared" si="0"/>

</xml_diff>